<commit_message>
Work for making demo data displayed
</commit_message>
<xml_diff>
--- a/kc_app/static/kc_app/files/example.xlsx
+++ b/kc_app/static/kc_app/files/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaboi/Desktop/Oaklab/KClusterInterface/kc_app/static/kc_app/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B412BB0-6992-7942-BBDB-6BAF2BE3B0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD1C878-CC0A-A347-A1D6-580BB3997096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1 - mock_kc_results" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="22">
-  <si>
-    <t>mock_kc_results</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>id</t>
   </si>
@@ -37,109 +34,116 @@
     <t>answerKey</t>
   </si>
   <si>
-    <t>skillref</t>
-  </si>
-  <si>
-    <t>step-name</t>
-  </si>
-  <si>
-    <t>ds-step-name</t>
-  </si>
-  <si>
-    <t>KC</t>
-  </si>
-  <si>
-    <t>elearning-mcq-1</t>
-  </si>
-  <si>
     <t>Multiple Choice</t>
   </si>
   <si>
-    <t>Which cognitive process aims to limit stress on working memory by fostering a deeper understanding of the content and learner engagement?
-a) Essential processing
-b) Extraneous processing
-c) Generative processing
-d) Limited capacity
-Answer: c</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>distinguish_tech_vs_lrng_centrd_lrng_vs_instrctn_skill</t>
-  </si>
-  <si>
-    <t>q2_distinguish_tech_lrnr_intrct_3_cog_pool_c968fda3fa664b3ebbb36d3bae128666</t>
-  </si>
-  <si>
-    <t>Activity gltl7_distinguish_tech_lrnr_intrct_3_4yxxf, part c968fda3fa664b3ebbb36d3bae128666 Multiple choice submission</t>
-  </si>
-  <si>
-    <t>!</t>
-  </si>
-  <si>
-    <t>elearning-mcq-2</t>
-  </si>
-  <si>
-    <t>Adding practice activities or relevant visuals are techniques used to increase psychological engagement as an attempt to
-a) Increase generative processing
-b) Increase essential processing
-c) Reduce extraneous processing
-Answer: a</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>q3_distinguish_tech_lrnr_intrct_3_cog_pool_b3423f78f89f49688e1e55b3ab9a7133</t>
-  </si>
-  <si>
-    <t>Activity gltl7_distinguish_tech_lrnr_intrct_3_u9usm, part b3423f78f89f49688e1e55b3ab9a7133 Multiple choice submission</t>
+    <t>choice_a</t>
+  </si>
+  <si>
+    <t>choice_b</t>
+  </si>
+  <si>
+    <t>choice_c</t>
+  </si>
+  <si>
+    <t>sciqa-2327</t>
+  </si>
+  <si>
+    <t>Which is more flexible?</t>
+  </si>
+  <si>
+    <t>Diamond</t>
+  </si>
+  <si>
+    <t>Wool Sweater</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>Compare properties of materials</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>natural science</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>grade3</t>
+  </si>
+  <si>
+    <t>spacing-1161-fib-5</t>
+  </si>
+  <si>
+    <t>Fill in the Blank</t>
+  </si>
+  <si>
+    <t>When forces are _____, an object’s motion does not change.</t>
+  </si>
+  <si>
+    <t>balanced</t>
+  </si>
+  <si>
+    <t>6.3 Force and Motion</t>
+  </si>
+  <si>
+    <t>Balance of forces</t>
+  </si>
+  <si>
+    <t>Forces</t>
+  </si>
+  <si>
+    <t>grade8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -149,106 +153,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -258,42 +172,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1455,696 +1345,588 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="140.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="65" style="1" customWidth="1"/>
-    <col min="6" max="6" width="140.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="166.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.33203125" style="1"/>
+    <col min="1" max="1" width="15.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13" style="2" customWidth="1"/>
+    <col min="3" max="3" width="110.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="11.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="65" style="2" customWidth="1"/>
+    <col min="9" max="9" width="140.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="166.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="80.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="K2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="7"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="7"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="7"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="7"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="7"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="7"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="7"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="7"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="7"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="7"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="7"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="L2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" ht="92" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" ht="68" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="92" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="92" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="92" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="92" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="92" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="92" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="92" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>